<commit_message>
Assembly in real world is done and some Joints CAD are modified
</commit_message>
<xml_diff>
--- a/Printed Parts Records/Sum_of_printed_Material.xlsx
+++ b/Printed Parts Records/Sum_of_printed_Material.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kulde\OneDrive\Desktop\Romeo_007\Printed Parts Records\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A8B581C-6127-42F9-BE17-669B7D374283}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44DD0279-E107-4089-8A29-706658C595F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12710" yWindow="0" windowWidth="12980" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="12980" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -52,6 +52,27 @@
   </si>
   <si>
     <t>PLA(Orange)</t>
+  </si>
+  <si>
+    <t>PLA(Brown)</t>
+  </si>
+  <si>
+    <t>ABS(Green)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unltimater </t>
+  </si>
+  <si>
+    <t>PLA(yellow)</t>
+  </si>
+  <si>
+    <t>PLA(Organge)</t>
+  </si>
+  <si>
+    <t>PLA (Yellow)</t>
+  </si>
+  <si>
+    <t>Creality</t>
   </si>
 </sst>
 </file>
@@ -375,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -472,6 +493,90 @@
         <v>20.6</v>
       </c>
     </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
+        <v>45985</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="1">
+        <v>348.26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="2">
+        <v>45987</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="1">
+        <v>273.31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="2">
+        <v>45988</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="1">
+        <v>881.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="2">
+        <v>45988</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="1">
+        <v>746.65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="2">
+        <v>45989</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="1">
+        <v>342.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="2">
+        <v>45991</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="1">
+        <v>126.7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Excel sheet updated + Airless tyres integrated
</commit_message>
<xml_diff>
--- a/Printed Parts Records/Sum_of_printed_Material.xlsx
+++ b/Printed Parts Records/Sum_of_printed_Material.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kulde\OneDrive\Desktop\Romeo_007\Printed Parts Records\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44DD0279-E107-4089-8A29-706658C595F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0520F0A-CDC1-4AB3-A666-939717D69352}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="12980" windowHeight="15370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
   <si>
     <t>Date</t>
   </si>
@@ -69,10 +69,43 @@
     <t>PLA(Organge)</t>
   </si>
   <si>
-    <t>PLA (Yellow)</t>
-  </si>
-  <si>
     <t>Creality</t>
+  </si>
+  <si>
+    <t>Purpose</t>
+  </si>
+  <si>
+    <t>Tolerance test of Extrusion</t>
+  </si>
+  <si>
+    <t>Pressfit Test</t>
+  </si>
+  <si>
+    <t>20*20 extrusion test</t>
+  </si>
+  <si>
+    <t>Servo motor case</t>
+  </si>
+  <si>
+    <t>Motor case print wasted</t>
+  </si>
+  <si>
+    <t>PLA (Blue)</t>
+  </si>
+  <si>
+    <t>Motor case printre used</t>
+  </si>
+  <si>
+    <t>front Sus joint + servo Link</t>
+  </si>
+  <si>
+    <t>PLA(blue)</t>
+  </si>
+  <si>
+    <t>threaded screws and joints</t>
+  </si>
+  <si>
+    <t>small Joints + Links</t>
   </si>
 </sst>
 </file>
@@ -396,19 +429,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="4" width="20.6328125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6328125" customWidth="1"/>
+    <col min="1" max="3" width="20.6328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.6328125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -419,11 +454,14 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>45939</v>
       </c>
@@ -433,11 +471,14 @@
       <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="1">
         <v>59.32</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>45939</v>
       </c>
@@ -447,11 +488,14 @@
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="1">
         <v>59.64</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>45940</v>
       </c>
@@ -461,11 +505,14 @@
       <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="1">
         <v>26.42</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>45940</v>
       </c>
@@ -475,11 +522,14 @@
       <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="1">
         <v>31.68</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>45941</v>
       </c>
@@ -489,11 +539,14 @@
       <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="1">
-        <v>20.6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="1">
+        <v>60.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>45985</v>
       </c>
@@ -503,25 +556,31 @@
       <c r="C7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="1">
         <v>348.26</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>45987</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="1">
-        <v>273.31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>45988</v>
       </c>
@@ -531,11 +590,14 @@
       <c r="C9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="1">
         <v>881.5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>45988</v>
       </c>
@@ -545,25 +607,31 @@
       <c r="C10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="1">
         <v>746.65</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>45989</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="1">
-        <v>342.5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="1">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>45991</v>
       </c>
@@ -573,7 +641,10 @@
       <c r="C12" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="1">
         <v>126.7</v>
       </c>
     </row>

</xml_diff>